<commit_message>
added interpolation to increase telemetry coordinate resolution for calculating deviation between real and target paths
</commit_message>
<xml_diff>
--- a/3scenarios/telemetry/PositionTelemetry_S1.xlsx
+++ b/3scenarios/telemetry/PositionTelemetry_S1.xlsx
@@ -17,13 +17,14 @@
     <sheet name="T8" sheetId="8" r:id="rId8"/>
     <sheet name="T9" sheetId="9" r:id="rId9"/>
     <sheet name="T10" sheetId="10" r:id="rId10"/>
+    <sheet name="Average Speed" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="5">
   <si>
     <t>X</t>
   </si>
@@ -35,6 +36,9 @@
   </si>
   <si>
     <t>Motion Profile Y</t>
+  </si>
+  <si>
+    <t>Scenario Average Speed (in/s)</t>
   </si>
 </sst>
 </file>
@@ -41824,6 +41828,32 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>32.70055697152094</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E253"/>

</xml_diff>